<commit_message>
RITM0032303 - suspend dward from github.battelleecology.org and remove dwardci from NEONScience ORG
</commit_message>
<xml_diff>
--- a/NEONScience/NEONScience_Users.xlsx
+++ b/NEONScience/NEONScience_Users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Common\CI\NEONScience\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhayes\git\NEONScience\NEONIT\NEONScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0993B889-F762-4D7E-9752-D075939C4C2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A158C32-8620-49B4-926A-8A6D521CC96E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="735" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4935" yWindow="3195" windowWidth="28770" windowHeight="16725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="github_users" sheetId="1" r:id="rId1"/>
@@ -754,9 +754,6 @@
     <t>stefanmet</t>
   </si>
   <si>
-    <t>Steve-Stone-Battelle</t>
-  </si>
-  <si>
     <t>StupendousMan67</t>
   </si>
   <si>
@@ -1343,6 +1340,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>removed 3/16</t>
   </si>
 </sst>
 </file>
@@ -2197,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,31 +2225,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>430</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2257,7 +2257,7 @@
         <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -2266,10 +2266,10 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2277,7 +2277,7 @@
         <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C3" t="s">
         <v>77</v>
@@ -2286,13 +2286,13 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2300,7 +2300,7 @@
         <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C4" t="s">
         <v>77</v>
@@ -2309,10 +2309,10 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
         <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C5" t="s">
         <v>77</v>
@@ -2332,10 +2332,10 @@
         <v>2019</v>
       </c>
       <c r="F5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
@@ -2355,10 +2355,10 @@
         <v>2015</v>
       </c>
       <c r="G6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>2015</v>
       </c>
       <c r="H7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
         <v>2015</v>
       </c>
       <c r="H8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>2015</v>
       </c>
       <c r="H9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2417,17 +2417,17 @@
         <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2435,16 +2435,16 @@
         <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2452,16 +2452,16 @@
         <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2469,19 +2469,19 @@
         <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2489,7 +2489,7 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
@@ -2498,10 +2498,10 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2509,19 +2509,19 @@
         <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2529,16 +2529,16 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2546,7 +2546,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -2555,10 +2555,10 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2566,16 +2566,16 @@
         <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D18" t="s">
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2583,22 +2583,22 @@
         <v>107</v>
       </c>
       <c r="B19" t="s">
+        <v>369</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
         <v>371</v>
       </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>372</v>
-      </c>
       <c r="G19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C20" t="s">
         <v>77</v>
@@ -2615,7 +2615,7 @@
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2623,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -2632,10 +2632,10 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2643,19 +2643,19 @@
         <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2663,19 +2663,19 @@
         <v>117</v>
       </c>
       <c r="B23" t="s">
+        <v>362</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>321</v>
+      </c>
+      <c r="G23" t="s">
         <v>363</v>
       </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>322</v>
-      </c>
-      <c r="G23" t="s">
-        <v>364</v>
-      </c>
       <c r="H23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2683,7 +2683,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2692,10 +2692,10 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H24" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2709,10 +2709,10 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2720,16 +2720,16 @@
         <v>122</v>
       </c>
       <c r="B26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D26" t="s">
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2737,7 +2737,7 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -2746,10 +2746,10 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H27" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2763,7 +2763,7 @@
         <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2771,7 +2771,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
@@ -2780,10 +2780,10 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2791,16 +2791,16 @@
         <v>128</v>
       </c>
       <c r="B30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D30" t="s">
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2808,7 +2808,7 @@
         <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C31" t="s">
         <v>47</v>
@@ -2817,10 +2817,10 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2828,7 +2828,7 @@
         <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C32" t="s">
         <v>77</v>
@@ -2837,10 +2837,10 @@
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2848,16 +2848,16 @@
         <v>140</v>
       </c>
       <c r="B33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D33" t="s">
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2879,7 +2879,7 @@
         <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C35" t="s">
         <v>77</v>
@@ -2888,7 +2888,7 @@
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>147</v>
       </c>
       <c r="B36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C36" t="s">
         <v>77</v>
@@ -2908,10 +2908,10 @@
         <v>2014</v>
       </c>
       <c r="F36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2919,19 +2919,19 @@
         <v>151</v>
       </c>
       <c r="B37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D37" t="s">
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2939,19 +2939,19 @@
         <v>153</v>
       </c>
       <c r="B38" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G38" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H38" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2959,7 +2959,7 @@
         <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C39" t="s">
         <v>51</v>
@@ -2968,10 +2968,10 @@
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2979,16 +2979,16 @@
         <v>160</v>
       </c>
       <c r="B40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H40" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C41" t="s">
         <v>55</v>
@@ -3005,10 +3005,10 @@
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3016,7 +3016,7 @@
         <v>170</v>
       </c>
       <c r="B42" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C42" t="s">
         <v>77</v>
@@ -3025,10 +3025,10 @@
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H42" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3036,7 +3036,7 @@
         <v>172</v>
       </c>
       <c r="B43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D43" t="s">
         <v>2</v>
@@ -3045,13 +3045,13 @@
         <v>2018</v>
       </c>
       <c r="F43" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
         <v>173</v>
       </c>
       <c r="B44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C44" t="s">
         <v>77</v>
@@ -3068,7 +3068,7 @@
         <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3076,7 +3076,7 @@
         <v>176</v>
       </c>
       <c r="B45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C45" t="s">
         <v>77</v>
@@ -3085,10 +3085,10 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H45" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
         <v>178</v>
       </c>
       <c r="B46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C46" t="s">
         <v>77</v>
@@ -3105,10 +3105,10 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
         <v>180</v>
       </c>
       <c r="B47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C47" t="s">
         <v>77</v>
@@ -3125,10 +3125,10 @@
         <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3136,19 +3136,19 @@
         <v>183</v>
       </c>
       <c r="B48" t="s">
+        <v>326</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
         <v>327</v>
       </c>
-      <c r="D48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" t="s">
-        <v>328</v>
-      </c>
       <c r="G48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3156,16 +3156,16 @@
         <v>188</v>
       </c>
       <c r="B49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3173,7 +3173,7 @@
         <v>190</v>
       </c>
       <c r="B50" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D50" t="s">
         <v>2</v>
@@ -3182,10 +3182,10 @@
         <v>2015</v>
       </c>
       <c r="F50" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H50" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3193,7 +3193,7 @@
         <v>201</v>
       </c>
       <c r="B51" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
@@ -3202,10 +3202,10 @@
         <v>2017</v>
       </c>
       <c r="F51" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3213,19 +3213,19 @@
         <v>205</v>
       </c>
       <c r="B52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D52" t="s">
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3233,7 +3233,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C53" t="s">
         <v>22</v>
@@ -3242,10 +3242,10 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H53" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3253,19 +3253,19 @@
         <v>209</v>
       </c>
       <c r="B54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G54" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H54" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3273,16 +3273,16 @@
         <v>217</v>
       </c>
       <c r="B55" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H55" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3290,19 +3290,19 @@
         <v>220</v>
       </c>
       <c r="B56" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D56" t="s">
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3310,16 +3310,16 @@
         <v>221</v>
       </c>
       <c r="B57" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D57" t="s">
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H57" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
         <v>224</v>
       </c>
       <c r="B58" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C58" t="s">
         <v>77</v>
@@ -3336,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="H58" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3344,7 +3344,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
@@ -3353,13 +3353,13 @@
         <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G59" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H59" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3367,16 +3367,16 @@
         <v>228</v>
       </c>
       <c r="B60" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H60" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3384,16 +3384,16 @@
         <v>229</v>
       </c>
       <c r="B61" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H61" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3401,16 +3401,16 @@
         <v>230</v>
       </c>
       <c r="B62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D62" t="s">
         <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H62" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3418,16 +3418,16 @@
         <v>231</v>
       </c>
       <c r="B63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H63" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3435,16 +3435,16 @@
         <v>233</v>
       </c>
       <c r="B64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D64" t="s">
         <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H64" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3452,7 +3452,7 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C65" t="s">
         <v>26</v>
@@ -3461,10 +3461,10 @@
         <v>2</v>
       </c>
       <c r="F65" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H65" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3472,16 +3472,16 @@
         <v>242</v>
       </c>
       <c r="B66" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D66" t="s">
         <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H66" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3489,19 +3489,19 @@
         <v>243</v>
       </c>
       <c r="B67" t="s">
+        <v>288</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+      <c r="F67" t="s">
+        <v>321</v>
+      </c>
+      <c r="G67" t="s">
         <v>289</v>
       </c>
-      <c r="D67" t="s">
-        <v>2</v>
-      </c>
-      <c r="F67" t="s">
-        <v>322</v>
-      </c>
-      <c r="G67" t="s">
-        <v>290</v>
-      </c>
       <c r="H67" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3509,7 +3509,7 @@
         <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -3518,52 +3518,52 @@
         <v>2</v>
       </c>
       <c r="F68" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H68" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B69" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D69" t="s">
         <v>2</v>
       </c>
       <c r="F69" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H69" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B70" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D70" t="s">
         <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H70" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B71" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C71" t="s">
         <v>77</v>
@@ -3572,24 +3572,24 @@
         <v>2</v>
       </c>
       <c r="H71" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D72" t="s">
         <v>2</v>
       </c>
       <c r="F72" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H72" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3606,7 +3606,7 @@
         <v>2018</v>
       </c>
       <c r="H73" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3623,7 +3623,7 @@
         <v>2018</v>
       </c>
       <c r="H74" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3631,7 +3631,7 @@
         <v>108</v>
       </c>
       <c r="B75" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C75" t="s">
         <v>77</v>
@@ -3643,10 +3643,10 @@
         <v>2017</v>
       </c>
       <c r="F75" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H75" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3654,7 +3654,7 @@
         <v>130</v>
       </c>
       <c r="B76" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C76" t="s">
         <v>77</v>
@@ -3666,10 +3666,10 @@
         <v>2014</v>
       </c>
       <c r="F76" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H76" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3677,7 +3677,7 @@
         <v>135</v>
       </c>
       <c r="B77" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C77" t="s">
         <v>77</v>
@@ -3689,10 +3689,10 @@
         <v>2015</v>
       </c>
       <c r="F77" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H77" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3700,19 +3700,19 @@
         <v>162</v>
       </c>
       <c r="B78" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D78" t="s">
         <v>31</v>
       </c>
       <c r="F78" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G78" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H78" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3720,7 +3720,7 @@
         <v>166</v>
       </c>
       <c r="B79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C79" t="s">
         <v>77</v>
@@ -3732,10 +3732,10 @@
         <v>2017</v>
       </c>
       <c r="F79" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H79" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3743,7 +3743,7 @@
         <v>202</v>
       </c>
       <c r="B80" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D80" t="s">
         <v>31</v>
@@ -3752,10 +3752,10 @@
         <v>2015</v>
       </c>
       <c r="F80" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H80" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3763,7 +3763,7 @@
         <v>203</v>
       </c>
       <c r="B81" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D81" t="s">
         <v>31</v>
@@ -3772,10 +3772,10 @@
         <v>2018</v>
       </c>
       <c r="F81" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3783,47 +3783,47 @@
         <v>239</v>
       </c>
       <c r="B82" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D82" t="s">
         <v>31</v>
       </c>
       <c r="F82" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G82" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H82" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>244</v>
+        <v>44</v>
       </c>
       <c r="B83" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D83" t="s">
         <v>31</v>
       </c>
       <c r="F83" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B84" t="s">
+        <v>277</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="D84" t="s">
         <v>31</v>
@@ -3832,12 +3832,12 @@
         <v>2018</v>
       </c>
       <c r="H84" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C85" t="s">
         <v>77</v>
@@ -3849,7 +3849,7 @@
         <v>2015</v>
       </c>
       <c r="H85" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3863,13 +3863,13 @@
         <v>2</v>
       </c>
       <c r="F86" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H86" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I86" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3877,7 +3877,7 @@
         <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C87" t="s">
         <v>30</v>
@@ -3886,13 +3886,13 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H87" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I87" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3900,16 +3900,16 @@
         <v>191</v>
       </c>
       <c r="B88" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
       </c>
       <c r="H88" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I88" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3917,7 +3917,7 @@
         <v>64</v>
       </c>
       <c r="B89" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C89" t="s">
         <v>65</v>
@@ -3926,13 +3926,13 @@
         <v>2</v>
       </c>
       <c r="F89" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H89" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I89" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C90" t="s">
         <v>20</v>
@@ -3949,13 +3949,13 @@
         <v>2</v>
       </c>
       <c r="F90" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H90" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I90" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3963,19 +3963,19 @@
         <v>206</v>
       </c>
       <c r="B91" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H91" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I91" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3983,36 +3983,36 @@
         <v>232</v>
       </c>
       <c r="B92" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D92" t="s">
         <v>2</v>
       </c>
       <c r="F92" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H92" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I92" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B93" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
       </c>
       <c r="H93" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I93" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4020,7 +4020,7 @@
         <v>82</v>
       </c>
       <c r="B94" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C94" t="s">
         <v>77</v>
@@ -4032,10 +4032,10 @@
         <v>2016</v>
       </c>
       <c r="H94" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I94" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4043,7 +4043,7 @@
         <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C95" t="s">
         <v>77</v>
@@ -4055,7 +4055,7 @@
         <v>2014</v>
       </c>
       <c r="F95" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4063,7 +4063,7 @@
         <v>86</v>
       </c>
       <c r="B96" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C96" t="s">
         <v>77</v>
@@ -4075,13 +4075,13 @@
         <v>2017</v>
       </c>
       <c r="G96" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H96" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I96" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4089,7 +4089,7 @@
         <v>102</v>
       </c>
       <c r="B97" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C97" t="s">
         <v>77</v>
@@ -4101,10 +4101,10 @@
         <v>2015</v>
       </c>
       <c r="H97" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I97" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4121,13 +4121,13 @@
         <v>2016</v>
       </c>
       <c r="F98" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H98" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I98" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4135,22 +4135,22 @@
         <v>115</v>
       </c>
       <c r="B99" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D99" t="s">
         <v>31</v>
       </c>
       <c r="F99" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G99" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H99" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I99" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4167,10 +4167,10 @@
         <v>2016</v>
       </c>
       <c r="H100" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I100" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,7 +4178,7 @@
         <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C101" t="s">
         <v>18</v>
@@ -4190,10 +4190,10 @@
         <v>2016</v>
       </c>
       <c r="H101" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I101" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4210,10 +4210,10 @@
         <v>2015</v>
       </c>
       <c r="H102" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I102" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>52</v>
       </c>
       <c r="B103" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C103" t="s">
         <v>53</v>
@@ -4233,13 +4233,13 @@
         <v>2019</v>
       </c>
       <c r="G103" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H103" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I103" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4247,22 +4247,22 @@
         <v>187</v>
       </c>
       <c r="B104" t="s">
+        <v>324</v>
+      </c>
+      <c r="C104" t="s">
+        <v>77</v>
+      </c>
+      <c r="D104" t="s">
+        <v>31</v>
+      </c>
+      <c r="G104" t="s">
         <v>325</v>
       </c>
-      <c r="C104" t="s">
-        <v>77</v>
-      </c>
-      <c r="D104" t="s">
-        <v>31</v>
-      </c>
-      <c r="G104" t="s">
-        <v>326</v>
-      </c>
       <c r="H104" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I104" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4279,18 +4279,18 @@
         <v>2015</v>
       </c>
       <c r="H105" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I105" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B106" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C106" t="s">
         <v>77</v>
@@ -4299,18 +4299,18 @@
         <v>31</v>
       </c>
       <c r="G106" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H106" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I106" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C107" t="s">
         <v>77</v>
@@ -4319,10 +4319,10 @@
         <v>31</v>
       </c>
       <c r="H107" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I107" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4330,7 +4330,7 @@
         <v>91</v>
       </c>
       <c r="B108" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C108" t="s">
         <v>77</v>
@@ -4339,7 +4339,7 @@
         <v>2</v>
       </c>
       <c r="H108" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4347,7 +4347,7 @@
         <v>15</v>
       </c>
       <c r="B109" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C109" t="s">
         <v>16</v>
@@ -4356,7 +4356,7 @@
         <v>2</v>
       </c>
       <c r="H109" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4364,7 +4364,7 @@
         <v>154</v>
       </c>
       <c r="B110" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C110" t="s">
         <v>77</v>
@@ -4376,10 +4376,10 @@
         <v>2018</v>
       </c>
       <c r="G110" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H110" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4387,7 +4387,7 @@
         <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C111" t="s">
         <v>57</v>
@@ -4399,10 +4399,10 @@
         <v>2018</v>
       </c>
       <c r="G111" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H111" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4410,7 +4410,7 @@
         <v>23</v>
       </c>
       <c r="B112" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C112" t="s">
         <v>24</v>
@@ -4419,7 +4419,7 @@
         <v>2</v>
       </c>
       <c r="H112" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4427,7 +4427,7 @@
         <v>7</v>
       </c>
       <c r="B113" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -4436,7 +4436,7 @@
         <v>2</v>
       </c>
       <c r="H113" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -4444,7 +4444,7 @@
         <v>36</v>
       </c>
       <c r="B114" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C114" t="s">
         <v>37</v>
@@ -4456,7 +4456,7 @@
         <v>2017</v>
       </c>
       <c r="H114" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4473,7 +4473,7 @@
         <v>2015</v>
       </c>
       <c r="H115" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4487,7 +4487,7 @@
         <v>2</v>
       </c>
       <c r="G116" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H116" t="s">
         <v>77</v>
@@ -4498,7 +4498,7 @@
         <v>81</v>
       </c>
       <c r="B117" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C117" t="s">
         <v>77</v>
@@ -4507,7 +4507,7 @@
         <v>2</v>
       </c>
       <c r="F117" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H117" t="s">
         <v>77</v>
@@ -4518,7 +4518,7 @@
         <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C118" t="s">
         <v>10</v>
@@ -4544,7 +4544,7 @@
         <v>2019</v>
       </c>
       <c r="G119" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H119" t="s">
         <v>77</v>
@@ -4555,7 +4555,7 @@
         <v>87</v>
       </c>
       <c r="B120" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C120" t="s">
         <v>77</v>
@@ -4572,7 +4572,7 @@
         <v>99</v>
       </c>
       <c r="B121" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C121" t="s">
         <v>77</v>
@@ -4581,7 +4581,7 @@
         <v>2</v>
       </c>
       <c r="E121" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H121" t="s">
         <v>77</v>
@@ -4592,7 +4592,7 @@
         <v>13</v>
       </c>
       <c r="B122" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C122" t="s">
         <v>14</v>
@@ -4609,7 +4609,7 @@
         <v>114</v>
       </c>
       <c r="B123" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C123" t="s">
         <v>77</v>
@@ -4618,7 +4618,7 @@
         <v>2</v>
       </c>
       <c r="F123" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H123" t="s">
         <v>77</v>
@@ -4635,7 +4635,7 @@
         <v>2</v>
       </c>
       <c r="G124" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H124" t="s">
         <v>77</v>
@@ -4697,7 +4697,7 @@
         <v>2</v>
       </c>
       <c r="E128" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H128" t="s">
         <v>77</v>
@@ -4725,7 +4725,7 @@
         <v>163</v>
       </c>
       <c r="B130" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C130" t="s">
         <v>77</v>
@@ -4754,7 +4754,7 @@
         <v>2017</v>
       </c>
       <c r="G131" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H131" t="s">
         <v>77</v>
@@ -4839,7 +4839,7 @@
         <v>2016</v>
       </c>
       <c r="G136" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H136" t="s">
         <v>77</v>
@@ -4856,7 +4856,7 @@
         <v>2</v>
       </c>
       <c r="E137" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H137" t="s">
         <v>77</v>
@@ -4884,7 +4884,7 @@
         <v>193</v>
       </c>
       <c r="B139" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C139" t="s">
         <v>77</v>
@@ -4893,7 +4893,7 @@
         <v>2</v>
       </c>
       <c r="E139" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H139" t="s">
         <v>77</v>
@@ -4921,7 +4921,7 @@
         <v>213</v>
       </c>
       <c r="B141" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C141" t="s">
         <v>77</v>
@@ -4933,7 +4933,7 @@
         <v>2015</v>
       </c>
       <c r="G141" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H141" t="s">
         <v>77</v>
@@ -4944,7 +4944,7 @@
         <v>66</v>
       </c>
       <c r="B142" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C142" t="s">
         <v>67</v>
@@ -4975,7 +4975,7 @@
         <v>223</v>
       </c>
       <c r="B144" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C144" t="s">
         <v>77</v>
@@ -5034,13 +5034,13 @@
         <v>234</v>
       </c>
       <c r="B148" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D148" t="s">
         <v>2</v>
       </c>
       <c r="F148" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H148" t="s">
         <v>77</v>
@@ -5076,19 +5076,19 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B151" t="s">
+        <v>285</v>
+      </c>
+      <c r="C151" t="s">
+        <v>77</v>
+      </c>
+      <c r="D151" t="s">
+        <v>2</v>
+      </c>
+      <c r="G151" t="s">
         <v>286</v>
-      </c>
-      <c r="C151" t="s">
-        <v>77</v>
-      </c>
-      <c r="D151" t="s">
-        <v>2</v>
-      </c>
-      <c r="G151" t="s">
-        <v>287</v>
       </c>
       <c r="H151" t="s">
         <v>77</v>
@@ -5099,7 +5099,7 @@
         <v>74</v>
       </c>
       <c r="B152" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C152" t="s">
         <v>75</v>
@@ -5108,7 +5108,7 @@
         <v>2</v>
       </c>
       <c r="G152" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H152" t="s">
         <v>77</v>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C153" t="s">
         <v>77</v>
@@ -5125,7 +5125,7 @@
         <v>2</v>
       </c>
       <c r="G153" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H153" t="s">
         <v>77</v>
@@ -5133,7 +5133,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C154" t="s">
         <v>77</v>
@@ -5142,7 +5142,7 @@
         <v>2</v>
       </c>
       <c r="G154" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H154" t="s">
         <v>77</v>
@@ -5150,10 +5150,10 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B155" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C155" t="s">
         <v>77</v>
@@ -5162,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="G155" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H155" t="s">
         <v>77</v>
@@ -5170,10 +5170,10 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B156" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C156" t="s">
         <v>77</v>
@@ -5182,7 +5182,7 @@
         <v>2</v>
       </c>
       <c r="E156" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H156" t="s">
         <v>77</v>
@@ -5193,16 +5193,16 @@
         <v>93</v>
       </c>
       <c r="B157" t="s">
+        <v>381</v>
+      </c>
+      <c r="C157" t="s">
+        <v>77</v>
+      </c>
+      <c r="D157" t="s">
+        <v>322</v>
+      </c>
+      <c r="E157" t="s">
         <v>382</v>
-      </c>
-      <c r="C157" t="s">
-        <v>77</v>
-      </c>
-      <c r="D157" t="s">
-        <v>323</v>
-      </c>
-      <c r="E157" t="s">
-        <v>383</v>
       </c>
       <c r="H157" t="s">
         <v>77</v>
@@ -5213,19 +5213,19 @@
         <v>127</v>
       </c>
       <c r="B158" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D158" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E158" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F158" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G158" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H158" t="s">
         <v>77</v>
@@ -5239,7 +5239,7 @@
         <v>77</v>
       </c>
       <c r="D159" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E159">
         <v>2019</v>
@@ -5250,16 +5250,16 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B160" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C160" t="s">
         <v>77</v>
       </c>
       <c r="D160" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H160" t="s">
         <v>77</v>
@@ -5284,7 +5284,7 @@
         <v>34</v>
       </c>
       <c r="B162" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C162" t="s">
         <v>35</v>
@@ -5293,7 +5293,7 @@
         <v>31</v>
       </c>
       <c r="G162" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H162" t="s">
         <v>77</v>
@@ -5304,7 +5304,7 @@
         <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C163" t="s">
         <v>77</v>
@@ -5316,7 +5316,7 @@
         <v>2016</v>
       </c>
       <c r="F163" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H163" t="s">
         <v>77</v>
@@ -5378,7 +5378,7 @@
         <v>97</v>
       </c>
       <c r="B167" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C167" t="s">
         <v>77</v>
@@ -5446,7 +5446,7 @@
         <v>42</v>
       </c>
       <c r="B171" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C171" t="s">
         <v>43</v>
@@ -5458,7 +5458,7 @@
         <v>2019</v>
       </c>
       <c r="G171" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H171" t="s">
         <v>77</v>
@@ -5486,7 +5486,7 @@
         <v>118</v>
       </c>
       <c r="B173" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C173" t="s">
         <v>77</v>
@@ -5540,7 +5540,7 @@
         <v>124</v>
       </c>
       <c r="B176" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C176" t="s">
         <v>77</v>
@@ -5552,7 +5552,7 @@
         <v>2016</v>
       </c>
       <c r="G176" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H176" t="s">
         <v>77</v>
@@ -5648,7 +5648,7 @@
         <v>137</v>
       </c>
       <c r="B182" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D182" t="s">
         <v>31</v>
@@ -5657,10 +5657,10 @@
         <v>2015</v>
       </c>
       <c r="F182" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G182" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H182" t="s">
         <v>77</v>
@@ -5671,7 +5671,7 @@
         <v>48</v>
       </c>
       <c r="B183" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C183" t="s">
         <v>49</v>
@@ -5759,7 +5759,7 @@
         <v>156</v>
       </c>
       <c r="B188" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D188" t="s">
         <v>31</v>
@@ -5768,10 +5768,10 @@
         <v>2016</v>
       </c>
       <c r="F188" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G188" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H188" t="s">
         <v>77</v>
@@ -5884,7 +5884,7 @@
         <v>58</v>
       </c>
       <c r="B195" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C195" t="s">
         <v>59</v>
@@ -5952,7 +5952,7 @@
         <v>60</v>
       </c>
       <c r="B199" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C199" t="s">
         <v>61</v>
@@ -5961,7 +5961,7 @@
         <v>31</v>
       </c>
       <c r="F199" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H199" t="s">
         <v>77</v>
@@ -6006,7 +6006,7 @@
         <v>62</v>
       </c>
       <c r="B202" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C202" t="s">
         <v>63</v>
@@ -6029,7 +6029,7 @@
         <v>31</v>
       </c>
       <c r="E203" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H203" t="s">
         <v>77</v>
@@ -6046,7 +6046,7 @@
         <v>31</v>
       </c>
       <c r="E204" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H204" t="s">
         <v>77</v>
@@ -6063,7 +6063,7 @@
         <v>2015</v>
       </c>
       <c r="F205" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H205" t="s">
         <v>77</v>
@@ -6193,7 +6193,7 @@
         <v>68</v>
       </c>
       <c r="B213" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C213" t="s">
         <v>69</v>
@@ -6244,7 +6244,7 @@
         <v>72</v>
       </c>
       <c r="B216" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C216" t="s">
         <v>73</v>
@@ -6256,7 +6256,7 @@
         <v>2016</v>
       </c>
       <c r="F216" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H216" t="s">
         <v>77</v>
@@ -6281,7 +6281,7 @@
         <v>238</v>
       </c>
       <c r="B218" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C218" t="s">
         <v>77</v>
@@ -6304,7 +6304,7 @@
         <v>31</v>
       </c>
       <c r="G219" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H219" t="s">
         <v>77</v>
@@ -6312,10 +6312,10 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B220" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C220" t="s">
         <v>77</v>
@@ -6329,7 +6329,7 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C221" t="s">
         <v>77</v>
@@ -6343,7 +6343,7 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C222" t="s">
         <v>77</v>
@@ -6352,7 +6352,7 @@
         <v>31</v>
       </c>
       <c r="E222" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H222" t="s">
         <v>77</v>
@@ -6360,7 +6360,7 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C223" t="s">
         <v>77</v>
@@ -6374,7 +6374,7 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C224" t="s">
         <v>77</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C225" t="s">
         <v>77</v>
@@ -6397,7 +6397,7 @@
         <v>31</v>
       </c>
       <c r="F225" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H225" t="s">
         <v>77</v>
@@ -6405,7 +6405,7 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C226" t="s">
         <v>77</v>
@@ -6422,13 +6422,13 @@
         <v>198</v>
       </c>
       <c r="B227" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C227" t="s">
         <v>77</v>
       </c>
       <c r="D227" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E227">
         <v>2017</v>
@@ -6442,7 +6442,7 @@
         <v>204</v>
       </c>
       <c r="D228" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E228">
         <v>2016</v>

</xml_diff>

<commit_message>
RITM0036083 - Set acrall to inactive.  She has left the company
</commit_message>
<xml_diff>
--- a/NEONScience/NEONScience_Users.xlsx
+++ b/NEONScience/NEONScience_Users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhayes\git\NEONScience\NEONIT\NEONScience\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhayes/git/NEONIT/NEONScience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A158C32-8620-49B4-926A-8A6D521CC96E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E2F722-780B-7C47-8D3C-4052A2B95FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="3195" windowWidth="28770" windowHeight="16725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="3200" windowWidth="28780" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="github_users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="443">
   <si>
     <t>covesturtevant</t>
   </si>
@@ -1343,6 +1343,12 @@
   </si>
   <si>
     <t>removed 3/16</t>
+  </si>
+  <si>
+    <t>does not work at Battelle any longer</t>
+  </si>
+  <si>
+    <t>Does not work at Battelle any longer</t>
   </si>
 </sst>
 </file>
@@ -2197,33 +2203,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>268</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -2272,7 +2278,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -2295,7 +2301,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -2395,7 +2401,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>218</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -2447,7 +2453,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -2464,7 +2470,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -2541,7 +2547,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>106</v>
       </c>
@@ -2578,7 +2584,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>107</v>
       </c>
@@ -2601,7 +2607,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -2618,7 +2624,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>116</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -2678,7 +2684,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2698,7 +2704,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -2715,7 +2721,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -2752,7 +2758,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>126</v>
       </c>
@@ -2766,7 +2772,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -2786,7 +2792,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>128</v>
       </c>
@@ -2803,7 +2809,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2823,7 +2829,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>138</v>
       </c>
@@ -2834,16 +2840,16 @@
         <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F32" t="s">
-        <v>321</v>
+        <v>442</v>
       </c>
       <c r="H32" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -2860,7 +2866,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>151</v>
       </c>
@@ -2934,7 +2940,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2974,7 +2980,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>160</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3011,7 +3017,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>170</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>172</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>173</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -3111,7 +3117,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>180</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>183</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>188</v>
       </c>
@@ -3168,7 +3174,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>190</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -3208,7 +3214,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>205</v>
       </c>
@@ -3228,7 +3234,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>21</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>209</v>
       </c>
@@ -3268,7 +3274,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>217</v>
       </c>
@@ -3285,7 +3291,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>220</v>
       </c>
@@ -3305,7 +3311,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>221</v>
       </c>
@@ -3322,7 +3328,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>224</v>
       </c>
@@ -3339,7 +3345,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>228</v>
       </c>
@@ -3379,7 +3385,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>229</v>
       </c>
@@ -3396,7 +3402,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>230</v>
       </c>
@@ -3413,7 +3419,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>231</v>
       </c>
@@ -3430,7 +3436,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>233</v>
       </c>
@@ -3447,7 +3453,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>25</v>
       </c>
@@ -3467,7 +3473,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>242</v>
       </c>
@@ -3484,7 +3490,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>243</v>
       </c>
@@ -3504,7 +3510,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>27</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>247</v>
       </c>
@@ -3541,7 +3547,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>256</v>
       </c>
@@ -3558,7 +3564,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>257</v>
       </c>
@@ -3575,7 +3581,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>264</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -3605,11 +3611,14 @@
       <c r="E73">
         <v>2018</v>
       </c>
+      <c r="G73" t="s">
+        <v>441</v>
+      </c>
       <c r="H73" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -3626,7 +3635,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>108</v>
       </c>
@@ -3649,7 +3658,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>130</v>
       </c>
@@ -3672,7 +3681,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>135</v>
       </c>
@@ -3695,7 +3704,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>162</v>
       </c>
@@ -3715,7 +3724,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>166</v>
       </c>
@@ -3738,7 +3747,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>202</v>
       </c>
@@ -3758,7 +3767,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>203</v>
       </c>
@@ -3778,7 +3787,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>239</v>
       </c>
@@ -3798,7 +3807,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -3815,7 +3824,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>255</v>
       </c>
@@ -3835,7 +3844,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>265</v>
       </c>
@@ -3852,7 +3861,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -3872,7 +3881,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -3895,7 +3904,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>191</v>
       </c>
@@ -3912,7 +3921,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>64</v>
       </c>
@@ -3935,7 +3944,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -3958,7 +3967,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -3978,7 +3987,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>232</v>
       </c>
@@ -3998,7 +4007,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>259</v>
       </c>
@@ -4015,7 +4024,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>82</v>
       </c>
@@ -4038,7 +4047,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>84</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>86</v>
       </c>
@@ -4084,7 +4093,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -4107,7 +4116,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -4130,7 +4139,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -4153,7 +4162,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>125</v>
       </c>
@@ -4173,7 +4182,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>17</v>
       </c>
@@ -4196,7 +4205,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>161</v>
       </c>
@@ -4216,7 +4225,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>52</v>
       </c>
@@ -4242,7 +4251,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>187</v>
       </c>
@@ -4265,7 +4274,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>210</v>
       </c>
@@ -4285,7 +4294,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>246</v>
       </c>
@@ -4308,7 +4317,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>251</v>
       </c>
@@ -4325,7 +4334,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>91</v>
       </c>
@@ -4342,7 +4351,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -4359,7 +4368,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>154</v>
       </c>
@@ -4382,7 +4391,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>56</v>
       </c>
@@ -4405,7 +4414,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>23</v>
       </c>
@@ -4422,7 +4431,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -4439,7 +4448,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>36</v>
       </c>
@@ -4459,7 +4468,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>146</v>
       </c>
@@ -4476,7 +4485,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>79</v>
       </c>
@@ -4493,7 +4502,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>81</v>
       </c>
@@ -4513,7 +4522,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -4530,7 +4539,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>85</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>87</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>99</v>
       </c>
@@ -4587,7 +4596,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -4604,7 +4613,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>114</v>
       </c>
@@ -4624,7 +4633,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -4641,7 +4650,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -4658,7 +4667,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>144</v>
       </c>
@@ -4672,7 +4681,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>152</v>
       </c>
@@ -4686,7 +4695,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>155</v>
       </c>
@@ -4703,7 +4712,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>157</v>
       </c>
@@ -4720,7 +4729,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>163</v>
       </c>
@@ -4740,7 +4749,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>164</v>
       </c>
@@ -4760,7 +4769,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>168</v>
       </c>
@@ -4777,7 +4786,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>175</v>
       </c>
@@ -4794,7 +4803,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>177</v>
       </c>
@@ -4808,7 +4817,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>181</v>
       </c>
@@ -4825,7 +4834,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>182</v>
       </c>
@@ -4845,7 +4854,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>185</v>
       </c>
@@ -4862,7 +4871,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>192</v>
       </c>
@@ -4879,7 +4888,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>193</v>
       </c>
@@ -4899,7 +4908,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>195</v>
       </c>
@@ -4916,7 +4925,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>213</v>
       </c>
@@ -4939,7 +4948,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>66</v>
       </c>
@@ -4956,7 +4965,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>222</v>
       </c>
@@ -4970,7 +4979,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>223</v>
       </c>
@@ -4987,7 +4996,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>225</v>
       </c>
@@ -5001,7 +5010,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>226</v>
       </c>
@@ -5015,7 +5024,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>227</v>
       </c>
@@ -5029,7 +5038,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>234</v>
       </c>
@@ -5046,7 +5055,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>236</v>
       </c>
@@ -5060,7 +5069,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>241</v>
       </c>
@@ -5074,7 +5083,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>245</v>
       </c>
@@ -5094,7 +5103,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>74</v>
       </c>
@@ -5114,7 +5123,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>253</v>
       </c>
@@ -5131,7 +5140,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>258</v>
       </c>
@@ -5148,7 +5157,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>261</v>
       </c>
@@ -5168,7 +5177,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>262</v>
       </c>
@@ -5188,7 +5197,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>93</v>
       </c>
@@ -5208,7 +5217,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>127</v>
       </c>
@@ -5231,7 +5240,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>189</v>
       </c>
@@ -5248,7 +5257,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>248</v>
       </c>
@@ -5265,7 +5274,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>76</v>
       </c>
@@ -5279,7 +5288,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>34</v>
       </c>
@@ -5299,7 +5308,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>83</v>
       </c>
@@ -5322,7 +5331,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>89</v>
       </c>
@@ -5339,7 +5348,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>92</v>
       </c>
@@ -5356,7 +5365,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>94</v>
       </c>
@@ -5373,7 +5382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>97</v>
       </c>
@@ -5390,7 +5399,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>100</v>
       </c>
@@ -5407,7 +5416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>101</v>
       </c>
@@ -5424,7 +5433,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>105</v>
       </c>
@@ -5441,7 +5450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>42</v>
       </c>
@@ -5464,7 +5473,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>110</v>
       </c>
@@ -5481,7 +5490,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>118</v>
       </c>
@@ -5501,7 +5510,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>120</v>
       </c>
@@ -5518,7 +5527,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>123</v>
       </c>
@@ -5535,7 +5544,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>124</v>
       </c>
@@ -5558,7 +5567,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>129</v>
       </c>
@@ -5575,7 +5584,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>131</v>
       </c>
@@ -5592,7 +5601,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>132</v>
       </c>
@@ -5609,7 +5618,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>133</v>
       </c>
@@ -5626,7 +5635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>136</v>
       </c>
@@ -5643,7 +5652,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>137</v>
       </c>
@@ -5666,7 +5675,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -5686,7 +5695,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>143</v>
       </c>
@@ -5703,7 +5712,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>148</v>
       </c>
@@ -5720,7 +5729,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>149</v>
       </c>
@@ -5737,7 +5746,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>150</v>
       </c>
@@ -5754,7 +5763,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>156</v>
       </c>
@@ -5777,7 +5786,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>158</v>
       </c>
@@ -5794,7 +5803,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>159</v>
       </c>
@@ -5811,7 +5820,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>165</v>
       </c>
@@ -5828,7 +5837,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>167</v>
       </c>
@@ -5845,7 +5854,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>171</v>
       </c>
@@ -5862,7 +5871,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>174</v>
       </c>
@@ -5879,7 +5888,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>58</v>
       </c>
@@ -5896,7 +5905,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>179</v>
       </c>
@@ -5913,7 +5922,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>184</v>
       </c>
@@ -5930,7 +5939,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>186</v>
       </c>
@@ -5947,7 +5956,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>60</v>
       </c>
@@ -5967,7 +5976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>194</v>
       </c>
@@ -5984,7 +5993,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>196</v>
       </c>
@@ -6001,7 +6010,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>62</v>
       </c>
@@ -6018,7 +6027,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>197</v>
       </c>
@@ -6035,7 +6044,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>200</v>
       </c>
@@ -6052,7 +6061,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>207</v>
       </c>
@@ -6069,7 +6078,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>208</v>
       </c>
@@ -6086,7 +6095,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>211</v>
       </c>
@@ -6103,7 +6112,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>212</v>
       </c>
@@ -6120,7 +6129,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>214</v>
       </c>
@@ -6137,7 +6146,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>215</v>
       </c>
@@ -6154,7 +6163,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>216</v>
       </c>
@@ -6171,7 +6180,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>219</v>
       </c>
@@ -6188,7 +6197,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>68</v>
       </c>
@@ -6208,7 +6217,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>70</v>
       </c>
@@ -6225,7 +6234,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>235</v>
       </c>
@@ -6239,7 +6248,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>72</v>
       </c>
@@ -6262,7 +6271,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>237</v>
       </c>
@@ -6276,7 +6285,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>238</v>
       </c>
@@ -6293,7 +6302,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>240</v>
       </c>
@@ -6310,7 +6319,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>244</v>
       </c>
@@ -6327,7 +6336,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>249</v>
       </c>
@@ -6341,7 +6350,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>250</v>
       </c>
@@ -6358,7 +6367,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>252</v>
       </c>
@@ -6372,7 +6381,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>254</v>
       </c>
@@ -6386,7 +6395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>260</v>
       </c>
@@ -6403,7 +6412,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>263</v>
       </c>
@@ -6417,7 +6426,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>198</v>
       </c>
@@ -6437,7 +6446,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>204</v>
       </c>

</xml_diff>